<commit_message>
Built out UV Analysis
Run everything with a folder name and AnalyzeUV
</commit_message>
<xml_diff>
--- a/UV Vis 150630/Directory.xlsx
+++ b/UV Vis 150630/Directory.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\Provincial_Bluffs\UV Vis 150630\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17630" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18620" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -127,7 +125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -162,7 +160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,7 +337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -350,15 +348,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="str">
         <f>D3&amp;$D$1</f>
         <v>0PRE.CSV</v>
@@ -367,7 +365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="str">
         <f>D4&amp;$D$2</f>
         <v>0POST.CSV</v>
@@ -376,7 +374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="str">
         <f>D5&amp;$D$1</f>
         <v>100PRE.CSV</v>
@@ -385,16 +383,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" t="str">
-        <f>D6&amp;$D$2</f>
+        <f>D5&amp;$D$2</f>
         <v>100POST.CSV</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="str">
         <f>D7&amp;$D$1</f>
         <v>200PRE.CSV</v>
@@ -403,7 +401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" t="str">
         <f>D8&amp;$D$2</f>
         <v>200POST.CSV</v>
@@ -412,7 +410,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" t="str">
         <f>D9&amp;$D$1</f>
         <v>300PRE.CSV</v>
@@ -421,7 +419,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" t="str">
         <f>D10&amp;$D$2</f>
         <v>300POST.CSV</v>
@@ -430,7 +428,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" t="str">
         <f>D11&amp;$D$1</f>
         <v>400PRE.CSV</v>
@@ -439,7 +437,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" t="str">
         <f>D12&amp;$D$2</f>
         <v>400POST.CSV</v>
@@ -448,7 +446,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" t="str">
         <f>D13&amp;$D$1</f>
         <v>500PRE.CSV</v>
@@ -457,7 +455,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" t="str">
         <f>D14&amp;$D$2</f>
         <v>500POST.CSV</v>
@@ -466,7 +464,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" t="str">
         <f>D15&amp;$D$1</f>
         <v>600PRE.CSV</v>
@@ -475,7 +473,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" t="str">
         <f>D16&amp;$D$2</f>
         <v>600POST.CSV</v>
@@ -484,7 +482,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" t="str">
         <f>D17&amp;$D$1</f>
         <v>700PRE.CSV</v>
@@ -493,7 +491,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" t="str">
         <f>D18&amp;$D$2</f>
         <v>700POST.CSV</v>
@@ -502,17 +500,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4">
       <c r="D17">
         <v>700</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4">
       <c r="D18">
         <v>700</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>